<commit_message>
Correction in TSR formula
</commit_message>
<xml_diff>
--- a/test/fuzzy_extractor/fuzzy_extractor_standard.xlsx
+++ b/test/fuzzy_extractor/fuzzy_extractor_standard.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Andrea\Desktop\Main\City\Individual Project\Source code\test\fuzzy_extractor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5690F28-4DFA-48F2-B90E-4376000E9F23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8361A1A9-B3A7-40D2-865C-BC9E473BD458}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -535,7 +535,7 @@
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -618,8 +618,8 @@
         <v>0</v>
       </c>
       <c r="F4" s="6">
-        <f xml:space="preserve"> SUM(1, -E4, -D4)</f>
-        <v>0</v>
+        <f xml:space="preserve"> (5 * SUM(1, -E4) + 4 * SUM(1, -D4)) / 9</f>
+        <v>0.55555555555555558</v>
       </c>
       <c r="G4" s="10" t="s">
         <v>10</v>
@@ -643,8 +643,8 @@
         <v>0</v>
       </c>
       <c r="F5" s="6">
-        <f xml:space="preserve"> SUM(1, -E5, -D5)</f>
-        <v>0</v>
+        <f t="shared" ref="F5:F6" si="0" xml:space="preserve"> (5 * SUM(1, -E5) + 4 * SUM(1, -D5)) / 9</f>
+        <v>0.55555555555555558</v>
       </c>
       <c r="G5" s="10" t="s">
         <v>10</v>
@@ -666,8 +666,8 @@
         <v>0.35339999999999999</v>
       </c>
       <c r="F6" s="6">
-        <f xml:space="preserve"> SUM(1, -E6, -D6)</f>
-        <v>1.2300000000000089E-2</v>
+        <f t="shared" si="0"/>
+        <v>0.52175555555555553</v>
       </c>
       <c r="G6" s="5">
         <v>1.5465317805555501</v>

</xml_diff>